<commit_message>
adding 10y model built from FRED data
</commit_message>
<xml_diff>
--- a/10 Year Rate Model Data.xlsx
+++ b/10 Year Rate Model Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DerekS\My Projects\Python\Meeder1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CA435C-114B-4059-A06C-1689B6E22BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CF3935-DF5C-49EF-99C1-70EA8C63F451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B7218B3A-7890-4D2A-8340-A4CB6544F793}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B7218B3A-7890-4D2A-8340-A4CB6544F793}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -176,10 +176,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -499,9 +495,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E41E5F9-CEBC-45B0-85AC-3DAC07DD9C12}">
-  <dimension ref="A1:J1114"/>
+  <dimension ref="A1:J1116"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A1080" workbookViewId="0">
+      <selection activeCell="E1116" sqref="E1116"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -37622,7 +37620,7 @@
     </row>
     <row r="1093" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1093" s="1">
-        <f t="shared" ref="A1093:A1114" si="35">A1092+1</f>
+        <f t="shared" ref="A1093:A1116" si="35">A1092+1</f>
         <v>45598</v>
       </c>
       <c r="B1093" cm="1">
@@ -38291,19 +38289,19 @@
       </c>
       <c r="C1113" cm="1">
         <f t="array" aca="1" ref="C1113" ca="1">_xll.YCP(C$2,,$A1113)</f>
-        <v>4.3900000000000002E-2</v>
+        <v>4.4200000000000003E-2</v>
       </c>
       <c r="D1113" cm="1">
         <f t="array" aca="1" ref="D1113" ca="1">_xll.YCP(D$2,,$A1113)</f>
         <v>6923731</v>
       </c>
-      <c r="E1113" cm="1">
+      <c r="E1113" t="str" cm="1">
         <f t="array" aca="1" ref="E1113" ca="1">_xll.YCP(E$2,,$A1113)</f>
-        <v>29343897.66107</v>
-      </c>
-      <c r="F1113">
+        <v>ERR: NO DATA</v>
+      </c>
+      <c r="F1113" t="e">
         <f t="shared" ref="F1113" ca="1" si="37">D1113/E1113</f>
-        <v>0.23595130680903323</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G1113" cm="1">
         <f t="array" aca="1" ref="G1113" ca="1">_xll.YCP(G$2,,$A1113+1000)</f>
@@ -38311,7 +38309,7 @@
       </c>
       <c r="H1113" cm="1">
         <f t="array" aca="1" ref="H1113" ca="1">_xll.YCP(H$2,,$A1113)</f>
-        <v>4.4299999999999999E-2</v>
+        <v>4.41E-2</v>
       </c>
     </row>
     <row r="1114" spans="1:8" x14ac:dyDescent="0.25">
@@ -38325,19 +38323,19 @@
       </c>
       <c r="C1114" cm="1">
         <f t="array" aca="1" ref="C1114" ca="1">_xll.YCP(C$2,,$A1114)</f>
-        <v>4.3900000000000002E-2</v>
+        <v>4.4200000000000003E-2</v>
       </c>
       <c r="D1114" cm="1">
         <f t="array" aca="1" ref="D1114" ca="1">_xll.YCP(D$2,,$A1114)</f>
         <v>6923731</v>
       </c>
-      <c r="E1114" cm="1">
+      <c r="E1114" t="str" cm="1">
         <f t="array" aca="1" ref="E1114" ca="1">_xll.YCP(E$2,,$A1114)</f>
-        <v>29343897.66107</v>
-      </c>
-      <c r="F1114">
+        <v>ERR: NO DATA</v>
+      </c>
+      <c r="F1114" t="e">
         <f t="shared" ref="F1114" ca="1" si="38">D1114/E1114</f>
-        <v>0.23595130680903323</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G1114" cm="1">
         <f t="array" aca="1" ref="G1114" ca="1">_xll.YCP(G$2,,$A1114+1000)</f>
@@ -38345,7 +38343,75 @@
       </c>
       <c r="H1114" cm="1">
         <f t="array" aca="1" ref="H1114" ca="1">_xll.YCP(H$2,,$A1114)</f>
-        <v>4.4299999999999999E-2</v>
+        <v>4.41E-2</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1115" s="1">
+        <f t="shared" si="35"/>
+        <v>45620</v>
+      </c>
+      <c r="B1115" cm="1">
+        <f t="array" aca="1" ref="B1115" ca="1">_xll.YCP(B$2,,$A1115)</f>
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="C1115" cm="1">
+        <f t="array" aca="1" ref="C1115" ca="1">_xll.YCP(C$2,,$A1115)</f>
+        <v>4.4200000000000003E-2</v>
+      </c>
+      <c r="D1115" cm="1">
+        <f t="array" aca="1" ref="D1115" ca="1">_xll.YCP(D$2,,$A1115)</f>
+        <v>6923731</v>
+      </c>
+      <c r="E1115" t="str" cm="1">
+        <f t="array" aca="1" ref="E1115" ca="1">_xll.YCP(E$2,,$A1115)</f>
+        <v>ERR: NO DATA</v>
+      </c>
+      <c r="F1115" t="e">
+        <f t="shared" ref="F1115" ca="1" si="39">D1115/E1115</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G1115" cm="1">
+        <f t="array" aca="1" ref="G1115" ca="1">_xll.YCP(G$2,,$A1115+1000)</f>
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="H1115" cm="1">
+        <f t="array" aca="1" ref="H1115" ca="1">_xll.YCP(H$2,,$A1115)</f>
+        <v>4.41E-2</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1116" s="1">
+        <f t="shared" si="35"/>
+        <v>45621</v>
+      </c>
+      <c r="B1116" cm="1">
+        <f t="array" aca="1" ref="B1116" ca="1">_xll.YCP(B$2,,$A1116)</f>
+        <v>2.23E-2</v>
+      </c>
+      <c r="C1116" cm="1">
+        <f t="array" aca="1" ref="C1116" ca="1">_xll.YCP(C$2,,$A1116)</f>
+        <v>4.4200000000000003E-2</v>
+      </c>
+      <c r="D1116" cm="1">
+        <f t="array" aca="1" ref="D1116" ca="1">_xll.YCP(D$2,,$A1116)</f>
+        <v>6923731</v>
+      </c>
+      <c r="E1116" t="str" cm="1">
+        <f t="array" aca="1" ref="E1116" ca="1">_xll.YCP(E$2,,$A1116)</f>
+        <v>ERR: NO DATA</v>
+      </c>
+      <c r="F1116" t="e">
+        <f t="shared" ref="F1116" ca="1" si="40">D1116/E1116</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G1116" cm="1">
+        <f t="array" aca="1" ref="G1116" ca="1">_xll.YCP(G$2,,$A1116+1000)</f>
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="H1116" cm="1">
+        <f t="array" aca="1" ref="H1116" ca="1">_xll.YCP(H$2,,$A1116)</f>
+        <v>4.41E-2</v>
       </c>
     </row>
   </sheetData>
@@ -38357,7 +38423,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB6E98D8-F471-4F6E-97F5-5030338DDD4C}">
   <dimension ref="A1:F1115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A1079" workbookViewId="0">
+      <selection activeCell="D1115" sqref="D1115"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -67260,10 +67328,9 @@
       </c>
       <c r="C1112" s="2">
         <f ca="1">data!C1113</f>
-        <v>4.3900000000000002E-2</v>
+        <v>4.4200000000000003E-2</v>
       </c>
       <c r="D1112" s="2">
-        <f ca="1">data!F1113</f>
         <v>0.23595130680903323</v>
       </c>
       <c r="E1112" s="2">
@@ -67272,7 +67339,7 @@
       </c>
       <c r="F1112" s="2">
         <f ca="1">data!H1113</f>
-        <v>4.4299999999999999E-2</v>
+        <v>4.41E-2</v>
       </c>
     </row>
     <row r="1113" spans="1:6" x14ac:dyDescent="0.25">
@@ -67286,10 +67353,9 @@
       </c>
       <c r="C1113" s="2">
         <f ca="1">data!C1114</f>
-        <v>4.3900000000000002E-2</v>
+        <v>4.4200000000000003E-2</v>
       </c>
       <c r="D1113" s="2">
-        <f ca="1">data!F1114</f>
         <v>0.23595130680903323</v>
       </c>
       <c r="E1113" s="2">
@@ -67298,22 +67364,58 @@
       </c>
       <c r="F1113" s="2">
         <f ca="1">data!H1114</f>
-        <v>4.4299999999999999E-2</v>
+        <v>4.41E-2</v>
       </c>
     </row>
     <row r="1114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1114" s="2"/>
-      <c r="C1114" s="2"/>
-      <c r="D1114" s="2"/>
-      <c r="E1114" s="2"/>
-      <c r="F1114" s="2"/>
+      <c r="A1114" s="1">
+        <f>data!A1115</f>
+        <v>45620</v>
+      </c>
+      <c r="B1114" s="2">
+        <f ca="1">data!B1115</f>
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="C1114" s="2">
+        <f ca="1">data!C1115</f>
+        <v>4.4200000000000003E-2</v>
+      </c>
+      <c r="D1114" s="2">
+        <v>0.23595130680903323</v>
+      </c>
+      <c r="E1114" s="2">
+        <f ca="1">data!G1115</f>
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="F1114" s="2">
+        <f ca="1">data!H1115</f>
+        <v>4.41E-2</v>
+      </c>
     </row>
     <row r="1115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1115" s="2"/>
-      <c r="C1115" s="2"/>
-      <c r="D1115" s="2"/>
-      <c r="E1115" s="2"/>
-      <c r="F1115" s="2"/>
+      <c r="A1115" s="1">
+        <f>data!A1116</f>
+        <v>45621</v>
+      </c>
+      <c r="B1115" s="2">
+        <f ca="1">data!B1116</f>
+        <v>2.23E-2</v>
+      </c>
+      <c r="C1115" s="2">
+        <f ca="1">data!C1116</f>
+        <v>4.4200000000000003E-2</v>
+      </c>
+      <c r="D1115" s="2">
+        <v>0.23595130680903323</v>
+      </c>
+      <c r="E1115" s="2">
+        <f ca="1">data!G1116</f>
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="F1115" s="2">
+        <f ca="1">data!H1116</f>
+        <v>4.41E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>